<commit_message>
Calcula incidencia de tipos de delitos por cada 100k
</commit_message>
<xml_diff>
--- a/INEI_2019-2023/INEI_poblacion_estimada_2019-2023.xlsx
+++ b/INEI_2019-2023/INEI_poblacion_estimada_2019-2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dial_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dial_\Documents\git-y-github\modelo-inseguridad-minds\INEI_2019-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEA0434C-AAC6-4934-870D-941F05321121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3820B38A-6D60-421F-BB54-CB6E2DA0B65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="72" windowWidth="14952" windowHeight="12168" xr2:uid="{DEFFAD69-4539-4CB9-A765-6EA6C7673E2F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DEFFAD69-4539-4CB9-A765-6EA6C7673E2F}"/>
   </bookViews>
   <sheets>
     <sheet name="INEI_poblacion_estimada_2019-20" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>junin</t>
   </si>
   <si>
-    <t>la_libertad</t>
-  </si>
-  <si>
     <t>lambayeque</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>loreto</t>
   </si>
   <si>
-    <t>madre_de_dios</t>
-  </si>
-  <si>
     <t>moquegua</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>puno</t>
   </si>
   <si>
-    <t>san_martin</t>
-  </si>
-  <si>
     <t>tacna</t>
   </si>
   <si>
@@ -119,6 +110,15 @@
   </si>
   <si>
     <t>ucayali</t>
+  </si>
+  <si>
+    <t>madre de dios</t>
+  </si>
+  <si>
+    <t>san martin</t>
+  </si>
+  <si>
+    <t>la libertad</t>
   </si>
 </sst>
 </file>
@@ -981,7 +981,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAF9E50-5CAE-498A-AE86-437131EF9430}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1312,7 +1314,7 @@
         <v>130000</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>1979901</v>
@@ -1335,7 +1337,7 @@
         <v>140000</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>1292105</v>
@@ -1358,7 +1360,7 @@
         <v>150000</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>10416139</v>
@@ -1381,7 +1383,7 @@
         <v>160000</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>1015212</v>
@@ -1404,7 +1406,7 @@
         <v>170000</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>167674</v>
@@ -1427,7 +1429,7 @@
         <v>180000</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>189781</v>
@@ -1450,7 +1452,7 @@
         <v>190000</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>272157</v>
@@ -1473,7 +1475,7 @@
         <v>200000</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>2013517</v>
@@ -1496,7 +1498,7 @@
         <v>210000</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23">
         <v>1239022</v>
@@ -1519,7 +1521,7 @@
         <v>220000</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>884283</v>
@@ -1542,7 +1544,7 @@
         <v>230000</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>363205</v>
@@ -1565,7 +1567,7 @@
         <v>240000</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>246699</v>
@@ -1588,7 +1590,7 @@
         <v>250000</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>574509</v>

</xml_diff>